<commit_message>
adding the other files that werent part of the original commit - enjoy!
</commit_message>
<xml_diff>
--- a/mini-v1.13 BOM.xlsx
+++ b/mini-v1.13 BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Part</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>MF-RES-0603-604K</t>
+  </si>
+  <si>
+    <t>10u 4mm</t>
+  </si>
+  <si>
+    <t>MF-CAP-4MM-10uF</t>
   </si>
 </sst>
 </file>
@@ -190,196 +196,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -737,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -807,129 +624,137 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="8" priority="15">
       <formula>"EXACT($F2,""x"")"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text=" ">
+    <cfRule type="containsText" dxfId="7" priority="13" operator="containsText" text=" ">
       <formula>NOT(ISERROR(SEARCH(" ",B6)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>"EXACT($F2,""x"")"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text=" ">
+      <formula>NOT(ISERROR(SEARCH(" ",B19)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>"EXACT($F2,""x"")"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text=" ">
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text=" ">
       <formula>NOT(ISERROR(SEARCH(" ",B18)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
-      <formula>"x"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>"EXACT($F2,""x"")"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text=" ">
-      <formula>NOT(ISERROR(SEARCH(" ",B17)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -937,15 +762,16 @@
     <hyperlink ref="B2" r:id="rId1" location="6partDetails" display="https://beta.macrofab.net/project/9qdpte - 6partDetails"/>
     <hyperlink ref="B3" r:id="rId2" tooltip="Open part details in a new window." display="https://beta.macrofab.net/part/MF-CAP-0603-1uF"/>
     <hyperlink ref="B4" r:id="rId3" tooltip="Open part details in a new window." display="https://beta.macrofab.net/part/MF-CAP-0603-0.1uF"/>
-    <hyperlink ref="B8" r:id="rId4" location="19partDetails" display="https://beta.macrofab.net/project/9qdpte/3 - 19partDetails"/>
-    <hyperlink ref="B10" r:id="rId5" location="22partDetails" display="https://beta.macrofab.net/project/9qdpte/3 - 22partDetails"/>
-    <hyperlink ref="B11" r:id="rId6" location="23partDetails" display="https://beta.macrofab.net/project/9qdpte/3 - 23partDetails"/>
-    <hyperlink ref="B13" r:id="rId7" location="24partDetails" display="https://beta.macrofab.net/project/9qdpte/3 - 24partDetails"/>
-    <hyperlink ref="B15" r:id="rId8" tooltip="Open part details in a new window." display="https://beta.macrofab.net/part/MF-DSC-SOT233-BSS138"/>
-    <hyperlink ref="B16" r:id="rId9" tooltip="Open part details in a new window." display="https://beta.macrofab.net/part/MF-SOT-235-3.3V-300mA"/>
-    <hyperlink ref="B9" r:id="rId10" location="21partDetails" display="https://beta.macrofab.net/project/9qdpte/4 - 21partDetails"/>
+    <hyperlink ref="B9" r:id="rId4" location="19partDetails" display="https://beta.macrofab.net/project/9qdpte/3 - 19partDetails"/>
+    <hyperlink ref="B11" r:id="rId5" location="22partDetails" display="https://beta.macrofab.net/project/9qdpte/3 - 22partDetails"/>
+    <hyperlink ref="B12" r:id="rId6" location="23partDetails" display="https://beta.macrofab.net/project/9qdpte/3 - 23partDetails"/>
+    <hyperlink ref="B14" r:id="rId7" location="24partDetails" display="https://beta.macrofab.net/project/9qdpte/3 - 24partDetails"/>
+    <hyperlink ref="B16" r:id="rId8" tooltip="Open part details in a new window." display="https://beta.macrofab.net/part/MF-DSC-SOT233-BSS138"/>
+    <hyperlink ref="B17" r:id="rId9" tooltip="Open part details in a new window." display="https://beta.macrofab.net/part/MF-SOT-235-3.3V-300mA"/>
+    <hyperlink ref="B10" r:id="rId10" location="21partDetails" display="https://beta.macrofab.net/project/9qdpte/4 - 21partDetails"/>
+    <hyperlink ref="B8" r:id="rId11" location="16partDetails" display="https://beta.macrofab.net/project/5xndt7 - 16partDetails"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>